<commit_message>
Update Delete File Double
</commit_message>
<xml_diff>
--- a/Data_Sepatu.xlsx
+++ b/Data_Sepatu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\html5.com\adudu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6985DC1-F22A-48F5-94F6-7FC387CFF5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534ACD9B-83AE-4684-B3AD-51C98FADCC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{013E588D-687E-4E80-8CF8-D7F5AC12605E}"/>
   </bookViews>
@@ -49,15 +49,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Size (UK)</t>
-  </si>
-  <si>
     <t>Beberapa pemain menarik perhatian. Tapi yang benar-benar hebat tak seperti itu, memecah kebisingan dengan sentuhan yang paling ringan. Fokus pada insting sepak bolamu dengan adidas Copa Sense. Foam Sensepoda mengisi setiap celah di bagian tumit sepatu bola untuk lapangan padat ini, yang membuatmu menyatu dengan upper berbahan K-leather yang lembut. Di bagian luar, tambahan bantalan Touchpods dan Softstuds membuatmu tetap fokus pada permainan.</t>
   </si>
   <si>
-    <t>SubDesc</t>
-  </si>
-  <si>
     <t>SEPATU BERBAHAN KULIT UNTUK SENTUHAN YANG SELEMBUT SUTRA.</t>
   </si>
   <si>
@@ -766,10 +760,16 @@
     <t>list_products/60.jpg</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>Stock</t>
+  </si>
+  <si>
+    <t>Sub Desc</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Image Path</t>
   </si>
 </sst>
 </file>
@@ -1172,9 +1172,8 @@
     <col min="3" max="3" width="50.77734375" customWidth="1"/>
     <col min="4" max="5" width="15.77734375" customWidth="1"/>
     <col min="6" max="6" width="60.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="7" max="8" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1188,19 +1187,19 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>243</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>5</v>
+        <v>244</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -1214,10 +1213,10 @@
         <v>2800000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>13</v>
@@ -1226,7 +1225,7 @@
         <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -1234,16 +1233,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>3200000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2">
         <v>11</v>
@@ -1252,7 +1251,7 @@
         <v>45</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -1260,16 +1259,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
         <v>1200000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2">
         <v>11</v>
@@ -1278,7 +1277,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -1286,16 +1285,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>3200000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="2">
         <v>11</v>
@@ -1304,7 +1303,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -1312,16 +1311,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
         <v>1200000</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" s="2">
         <v>12</v>
@@ -1330,7 +1329,7 @@
         <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
@@ -1338,16 +1337,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <v>1200000</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2">
         <v>13</v>
@@ -1356,7 +1355,7 @@
         <v>42</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -1364,16 +1363,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>4000000</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2">
         <v>12</v>
@@ -1382,7 +1381,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -1390,16 +1389,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2">
         <v>2200000</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2">
         <v>12</v>
@@ -1408,7 +1407,7 @@
         <v>44</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -1416,16 +1415,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>1300000</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2">
         <v>11</v>
@@ -1434,7 +1433,7 @@
         <v>38</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
@@ -1442,16 +1441,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>4000000</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2">
         <v>13</v>
@@ -1460,7 +1459,7 @@
         <v>35</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1468,16 +1467,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2">
         <v>1000000</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G13" s="2">
         <v>12</v>
@@ -1486,7 +1485,7 @@
         <v>42</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -1494,16 +1493,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>1900000</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G14" s="2">
         <v>11</v>
@@ -1512,7 +1511,7 @@
         <v>93</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
@@ -1520,16 +1519,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2">
         <v>1800000</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G15" s="2">
         <v>13</v>
@@ -1538,7 +1537,7 @@
         <v>99</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
@@ -1546,16 +1545,16 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2">
         <v>1700000</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2">
         <v>11</v>
@@ -1564,7 +1563,7 @@
         <v>34</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
@@ -1572,16 +1571,16 @@
         <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2">
         <v>900000</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2">
         <v>13</v>
@@ -1590,7 +1589,7 @@
         <v>32</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
@@ -1598,16 +1597,16 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="2">
         <v>1900000</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2">
         <v>12</v>
@@ -1616,7 +1615,7 @@
         <v>41</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
@@ -1624,16 +1623,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2">
         <v>2000000</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="2">
         <v>13</v>
@@ -1642,7 +1641,7 @@
         <v>39</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -1650,16 +1649,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="2">
         <v>700000</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G20" s="2">
         <v>11</v>
@@ -1668,7 +1667,7 @@
         <v>77</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
@@ -1676,16 +1675,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2">
         <v>2200000</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G21" s="2">
         <v>11</v>
@@ -1694,7 +1693,7 @@
         <v>30</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1702,16 +1701,16 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2">
         <v>3200000</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="2">
         <v>12</v>
@@ -1720,7 +1719,7 @@
         <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
@@ -1728,16 +1727,16 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="2">
         <v>2800000</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G23" s="2">
         <v>11</v>
@@ -1746,7 +1745,7 @@
         <v>53</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
@@ -1754,16 +1753,16 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2">
         <v>1800000</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" s="2">
         <v>11</v>
@@ -1772,7 +1771,7 @@
         <v>51</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
@@ -1780,16 +1779,16 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2">
         <v>3200000</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G25" s="2">
         <v>12</v>
@@ -1798,7 +1797,7 @@
         <v>42</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
@@ -1806,16 +1805,16 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="2">
         <v>3200000</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G26" s="2">
         <v>11</v>
@@ -1824,7 +1823,7 @@
         <v>35</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1832,16 +1831,16 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2">
         <v>3600000</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G27" s="2">
         <v>13</v>
@@ -1850,7 +1849,7 @@
         <v>54</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1858,16 +1857,16 @@
         <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28" s="2">
         <v>1600000</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G28" s="2">
         <v>13</v>
@@ -1876,7 +1875,7 @@
         <v>33</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1884,16 +1883,16 @@
         <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2">
         <v>1500000</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G29" s="2">
         <v>13</v>
@@ -1902,7 +1901,7 @@
         <v>43</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
@@ -1910,16 +1909,16 @@
         <v>28</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2">
         <v>2000000</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G30" s="2">
         <v>11</v>
@@ -1928,7 +1927,7 @@
         <v>31</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1936,16 +1935,16 @@
         <v>29</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" s="2">
         <v>3200000</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G31" s="2">
         <v>11</v>
@@ -1954,7 +1953,7 @@
         <v>37</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1962,16 +1961,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2">
         <v>800000</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G32" s="2">
         <v>12</v>
@@ -1980,7 +1979,7 @@
         <v>60</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
@@ -1988,16 +1987,16 @@
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D33" s="2">
         <v>1800000</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G33" s="2">
         <v>12</v>
@@ -2006,7 +2005,7 @@
         <v>34</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
@@ -2014,16 +2013,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" s="2">
         <v>2000000</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G34" s="2">
         <v>11</v>
@@ -2032,7 +2031,7 @@
         <v>99</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
@@ -2040,16 +2039,16 @@
         <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D35" s="2">
         <v>1900000</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G35" s="2">
         <v>13</v>
@@ -2058,7 +2057,7 @@
         <v>49</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
@@ -2066,16 +2065,16 @@
         <v>34</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D36" s="2">
         <v>1300000</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G36" s="2">
         <v>12</v>
@@ -2084,7 +2083,7 @@
         <v>32</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
@@ -2092,16 +2091,16 @@
         <v>35</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D37" s="2">
         <v>2200000</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G37" s="2">
         <v>13</v>
@@ -2110,7 +2109,7 @@
         <v>31</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
@@ -2118,16 +2117,16 @@
         <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D38" s="2">
         <v>1700000</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G38" s="2">
         <v>12</v>
@@ -2136,7 +2135,7 @@
         <v>82</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -2144,16 +2143,16 @@
         <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D39" s="2">
         <v>1800000</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G39" s="2">
         <v>13</v>
@@ -2162,7 +2161,7 @@
         <v>44</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
@@ -2170,16 +2169,16 @@
         <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" s="2">
         <v>1400000</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G40" s="2">
         <v>12</v>
@@ -2188,7 +2187,7 @@
         <v>54</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
@@ -2196,16 +2195,16 @@
         <v>39</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D41" s="2">
         <v>2100000</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G41" s="2">
         <v>13</v>
@@ -2214,7 +2213,7 @@
         <v>51</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
@@ -2222,16 +2221,16 @@
         <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D42" s="2">
         <v>1500000</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G42" s="2">
         <v>11</v>
@@ -2240,7 +2239,7 @@
         <v>55</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -2248,16 +2247,16 @@
         <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D43" s="2">
         <v>2200000</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G43" s="2">
         <v>12</v>
@@ -2266,7 +2265,7 @@
         <v>34</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
@@ -2274,16 +2273,16 @@
         <v>42</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D44" s="2">
         <v>1400000</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G44" s="2">
         <v>11</v>
@@ -2292,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
@@ -2300,16 +2299,16 @@
         <v>43</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D45" s="2">
         <v>1900000</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G45" s="2">
         <v>12</v>
@@ -2318,7 +2317,7 @@
         <v>91</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
@@ -2326,16 +2325,16 @@
         <v>44</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D46" s="2">
         <v>1100000</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G46" s="2">
         <v>13</v>
@@ -2344,7 +2343,7 @@
         <v>70</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
@@ -2352,16 +2351,16 @@
         <v>45</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="2">
         <v>800000</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G47" s="2">
         <v>11</v>
@@ -2370,7 +2369,7 @@
         <v>35</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
@@ -2378,16 +2377,16 @@
         <v>46</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D48" s="2">
         <v>1300000</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G48" s="2">
         <v>11</v>
@@ -2396,7 +2395,7 @@
         <v>31</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
@@ -2404,16 +2403,16 @@
         <v>47</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D49" s="2">
         <v>2300000</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G49" s="2">
         <v>11</v>
@@ -2422,7 +2421,7 @@
         <v>75</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
@@ -2430,16 +2429,16 @@
         <v>48</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D50" s="2">
         <v>1200000</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G50" s="2">
         <v>13</v>
@@ -2448,7 +2447,7 @@
         <v>58</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2456,16 +2455,16 @@
         <v>49</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D51" s="2">
         <v>1300000</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G51" s="2">
         <v>11</v>
@@ -2474,7 +2473,7 @@
         <v>35</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
@@ -2482,16 +2481,16 @@
         <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D52" s="2">
         <v>800000</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G52" s="2">
         <v>13</v>
@@ -2500,7 +2499,7 @@
         <v>51</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2508,16 +2507,16 @@
         <v>51</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D53" s="2">
         <v>800000</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G53" s="2">
         <v>13</v>
@@ -2526,7 +2525,7 @@
         <v>65</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
@@ -2534,16 +2533,16 @@
         <v>52</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D54" s="2">
         <v>1100000</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G54" s="2">
         <v>13</v>
@@ -2552,7 +2551,7 @@
         <v>78</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
@@ -2560,16 +2559,16 @@
         <v>53</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D55" s="2">
         <v>900000</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G55" s="2">
         <v>12</v>
@@ -2578,7 +2577,7 @@
         <v>69</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
@@ -2586,16 +2585,16 @@
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D56" s="2">
         <v>3000000</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G56" s="2">
         <v>11</v>
@@ -2604,7 +2603,7 @@
         <v>66</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
@@ -2612,16 +2611,16 @@
         <v>55</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D57" s="2">
         <v>2800000</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G57" s="2">
         <v>12</v>
@@ -2630,7 +2629,7 @@
         <v>52</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
@@ -2638,16 +2637,16 @@
         <v>56</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D58" s="2">
         <v>850000</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G58" s="2">
         <v>12</v>
@@ -2656,7 +2655,7 @@
         <v>39</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
@@ -2664,16 +2663,16 @@
         <v>57</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D59" s="2">
         <v>2200000</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G59" s="2">
         <v>13</v>
@@ -2682,7 +2681,7 @@
         <v>78</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
@@ -2690,16 +2689,16 @@
         <v>58</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D60" s="2">
         <v>2700000</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G60" s="2">
         <v>11</v>
@@ -2708,7 +2707,7 @@
         <v>31</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
@@ -2716,16 +2715,16 @@
         <v>59</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D61" s="2">
         <v>2560000</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G61" s="2">
         <v>12</v>
@@ -2734,7 +2733,7 @@
         <v>33</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2742,16 +2741,16 @@
         <v>60</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D62" s="2">
         <v>1400000</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G62" s="2">
         <v>11</v>
@@ -2760,7 +2759,7 @@
         <v>78</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>